<commit_message>
Comments added to HEREstats WMean
</commit_message>
<xml_diff>
--- a/CE599_JB_Project/Compare/Copy of HERE Data Formatter.xlsx
+++ b/CE599_JB_Project/Compare/Copy of HERE Data Formatter.xlsx
@@ -804,11 +804,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1166,7 +1166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BY11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:R11"/>
     </sheetView>
   </sheetViews>
@@ -1228,19 +1228,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:77" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
     </row>
     <row r="2" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -1495,7 +1495,7 @@
         <v>13.3547648306384</v>
       </c>
       <c r="G3">
-        <v>9.9437509586657296</v>
+        <v>11.0147556915277</v>
       </c>
       <c r="H3">
         <v>27.563776711455098</v>
@@ -1513,7 +1513,7 @@
         <v>16.3018327659885</v>
       </c>
       <c r="M3">
-        <v>9.8371965627188906</v>
+        <v>10.845823445326401</v>
       </c>
       <c r="N3">
         <v>29.231124598363699</v>
@@ -1528,7 +1528,7 @@
         <v>6.5614081954859804</v>
       </c>
       <c r="R3">
-        <v>10.3048566511512</v>
+        <v>11.7141004374893</v>
       </c>
       <c r="S3">
         <v>26.962004403339201</v>
@@ -1549,7 +1549,7 @@
         <v>25.4551928321895</v>
       </c>
       <c r="Y3">
-        <v>9.6078629097882295</v>
+        <v>10.6532579483576</v>
       </c>
       <c r="Z3">
         <v>29.7556802646872</v>
@@ -1567,7 +1567,7 @@
         <v>19.623512258671099</v>
       </c>
       <c r="AE3">
-        <v>9.9483545466127303</v>
+        <v>10.6817822447937</v>
       </c>
       <c r="AF3">
         <v>27.5768222844961</v>
@@ -1585,7 +1585,7 @@
         <v>30.532507626773601</v>
       </c>
       <c r="AK3">
-        <v>8.9877614633645297</v>
+        <v>10.09293556908</v>
       </c>
       <c r="AL3">
         <v>23.6272730392078</v>
@@ -1603,7 +1603,7 @@
         <v>30.696542284023401</v>
       </c>
       <c r="AQ3">
-        <v>9.49135268447837</v>
+        <v>10.6931989366949</v>
       </c>
       <c r="AR3">
         <v>1.49814308704371</v>
@@ -1762,64 +1762,64 @@
       </c>
     </row>
     <row r="6" spans="1:77" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <f>B3</f>
         <v>27.826300425367499</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <f>G3</f>
-        <v>9.9437509586657296</v>
-      </c>
-      <c r="D6" s="2">
+        <v>11.0147556915277</v>
+      </c>
+      <c r="D6" s="1">
         <f>E3</f>
         <v>14038.743128460201</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <f>F3</f>
         <v>13.3547648306384</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <f>C3</f>
         <v>37.854400724904103</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <f>D3</f>
         <v>11.2789483417427</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1">
         <f>AT3</f>
         <v>1.33410929703627</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="1">
         <f>AY3</f>
         <v>1.32579371319295</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1">
         <f>BD3</f>
         <v>1.42126182221138</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="1">
         <f>AU3</f>
         <v>3.5581460843956698</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="1">
         <f>AZ3</f>
         <v>3.30073295266196</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="1">
         <f>BE3</f>
         <v>3.90347252195025</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="1">
         <f>AV3</f>
         <v>1.62704014650496</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="1">
         <f>BA3</f>
         <v>1.47167750499804</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6" s="1">
         <f>BF3</f>
         <v>1.7231226469357499</v>
       </c>
@@ -1828,211 +1828,211 @@
       </c>
     </row>
     <row r="7" spans="1:77" x14ac:dyDescent="0.3">
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <f>H3</f>
         <v>27.563776711455098</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <f>M3</f>
-        <v>9.8371965627188906</v>
-      </c>
-      <c r="D7" s="2">
+        <v>10.845823445326401</v>
+      </c>
+      <c r="D7" s="1">
         <f>K3</f>
         <v>11925.223709412499</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <f>L3</f>
         <v>16.3018327659885</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <f>I3</f>
         <v>37.406630777814897</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <f>J3</f>
         <v>11.2750786271296</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1">
         <f>BG3</f>
         <v>1.3393454798767901</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="1">
         <f>BI3</f>
         <v>1.3202860673827801</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
         <f>BK3</f>
         <v>1.41741484873534</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="1">
         <f>BH3</f>
         <v>3.55385600769013</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="1">
         <f>BJ3</f>
         <v>3.2595710151749002</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="1">
         <f>BL3</f>
         <v>3.7744854660866598</v>
       </c>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
       <c r="R7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:77" x14ac:dyDescent="0.3">
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <f>N3</f>
         <v>29.231124598363699</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <f>R3</f>
-        <v>10.3048566511512</v>
-      </c>
-      <c r="D8" s="2">
+        <v>11.7141004374893</v>
+      </c>
+      <c r="D8" s="1">
         <f>P3</f>
         <v>1965.3264197866499</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <f>Q3</f>
         <v>6.5614081954859804</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <f>O3</f>
         <v>39.609113263759802</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
       <c r="R8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:77" x14ac:dyDescent="0.3">
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <f>Z3</f>
         <v>29.7556802646872</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <f>AK3</f>
-        <v>8.9877614633645297</v>
-      </c>
-      <c r="D9" s="2">
+        <v>10.09293556908</v>
+      </c>
+      <c r="D9" s="1">
         <f>AC3</f>
         <v>1794.3723678103099</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <f>X3</f>
         <v>25.4551928321895</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2">
+      <c r="F9" s="1"/>
+      <c r="G9" s="1">
         <f>AA3</f>
         <v>13.307915952424</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <f>T3</f>
         <v>29.737963896099501</v>
       </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
       <c r="R9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:77" x14ac:dyDescent="0.3">
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <f>AF3</f>
         <v>27.5768222844961</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <f>AK3</f>
-        <v>8.9877614633645297</v>
-      </c>
-      <c r="D10" s="2">
+        <v>10.09293556908</v>
+      </c>
+      <c r="D10" s="1">
         <f>AI3</f>
         <v>5583.8269712587198</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <f>AJ3</f>
         <v>30.532507626773601</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1">
         <f>AG3</f>
         <v>11.9091763203306</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <f>T3</f>
         <v>29.737963896099501</v>
       </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
       <c r="R10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:77" x14ac:dyDescent="0.3">
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <f>AL3</f>
         <v>23.6272730392078</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <f>AQ3</f>
-        <v>9.49135268447837</v>
-      </c>
-      <c r="D11" s="2">
+        <v>10.6931989366949</v>
+      </c>
+      <c r="D11" s="1">
         <f>AO3</f>
         <v>2806.8974155944902</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <f>AP3</f>
         <v>30.696542284023401</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2">
+      <c r="F11" s="1"/>
+      <c r="G11" s="1">
         <f>AM3</f>
         <v>9.3326968949189606</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <f>T3</f>
         <v>29.737963896099501</v>
       </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
       <c r="R11" t="s">
         <v>13</v>
       </c>

</xml_diff>